<commit_message>
Modify the backlog and update the README.md
</commit_message>
<xml_diff>
--- a/docs/Productbacklog_group58.xlsx
+++ b/docs/Productbacklog_group58.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C7A522-21D8-44E6-9EDB-8DEAB3D8090A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D5DEA-2D1A-4539-8287-AB2F10ADC326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3915" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="106">
   <si>
     <t>Story ID</t>
   </si>
@@ -489,6 +489,55 @@
     <t>1.Verify that system allows logged-in users to access and modify their profile information (e.g., name, email, phone number) from their account settings.
 2.Verify that users can click “Save” to update their profile, and the system confirms the update with a success message.
 3.Verify that the updated information is immediately reflected across the user’s account and any associated services.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>As an end user,
+I want a centralized menu with clear navigation buttons,
+So that I can efficiently access all core financial management modules.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">User Interface </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Verify that the main menu displays buttons for User Info/VIP/Charts/Cards/Transactions/Logout.
+2. Verify clicking buttons redirects to corresponding interfaces and back button returns to main menu."</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main Menu Navigation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIP Membership Recharge</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Financial Analysis System</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>As a premium user,
+I want to view my VIP status and recharge membership durations,
+So that I can unlock exclusive financial management benefits.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>As a budget-conscious user,
+I want visual charts showing spending categories and income/expense trends,
+So that I can make informed financial decisions based on data insights.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Verify pie chart displays expense categories from transaction.csv.
+2. Verify bar chart shows monthly trends and handles data loading errors.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Verify the interface displays VIP expiry dates and remaining days.
+2. Verify popup allows selecting 1/3/12-month plans and updates user.csv data.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -759,9 +808,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -773,6 +819,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1079,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="80.150000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1536,7 +1585,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="80.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14">
+      <c r="A17" s="13">
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -1675,7 +1724,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="80.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="16">
+      <c r="A22" s="15">
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -1704,7 +1753,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="80.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="17">
+      <c r="A23" s="16">
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -1733,35 +1782,118 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="80.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="11">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="8">
         <v>5</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="12" t="s">
+      <c r="H24" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I24" s="15" t="s">
+      <c r="I24" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="80.150000000000006" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:9" s="17" customFormat="1" ht="80.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="8">
+        <v>3</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="17" customFormat="1" ht="80.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="8">
+        <v>4</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="17" customFormat="1" ht="80.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="11">
+        <v>26</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="12">
+        <v>4</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="80.150000000000006" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>